<commit_message>
add function for training, add testing and visualization
</commit_message>
<xml_diff>
--- a/exp_notes.xlsx
+++ b/exp_notes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="281">
   <si>
     <r>
       <rPr>
@@ -6521,6 +6521,54 @@
   </si>
   <si>
     <t xml:space="preserve">Valacc=0.27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb_1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">随便试了各种参数，都不</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">work</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">3_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labeled data</t>
   </si>
 </sst>
 </file>
@@ -6533,7 +6581,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -6562,6 +6610,12 @@
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC Regular"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -6630,7 +6684,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6680,6 +6734,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6770,17 +6828,17 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.24696356275304"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.53441295546559"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="44.1336032388664"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="44.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8192,18 +8250,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:M12"/>
+  <dimension ref="A2:M21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L13" activeCellId="0" sqref="L13"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.3522267206478"/>
     <col collapsed="false" hidden="false" max="12" min="8" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="46.919028340081"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="47.2388663967611"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -8340,7 +8398,7 @@
       <c r="A9" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="C9" s="0" t="s">
         <v>264</v>
       </c>
       <c r="K9" s="0" t="n">
@@ -8355,11 +8413,11 @@
         <v>0.0001</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="C11" s="0" t="s">
         <v>267</v>
       </c>
       <c r="K11" s="0" t="n">
@@ -8378,6 +8436,53 @@
       </c>
       <c r="L12" s="0" t="s">
         <v>270</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
iterloader bug, save npy, more data_aug
</commit_message>
<xml_diff>
--- a/exp_notes.xlsx
+++ b/exp_notes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="388">
   <si>
     <r>
       <rPr>
@@ -6867,10 +6867,88 @@
     <t xml:space="preserve">8_1</t>
   </si>
   <si>
+    <t xml:space="preserve">0.06, 0.44, 0.24</t>
+  </si>
+  <si>
     <t xml:space="preserve">8_2</t>
   </si>
   <si>
     <t xml:space="preserve">data_aug for labeled too</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.40, 0.45, 0.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">another loss define by diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.30, 0.39, 0.26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.37, 0.42, 0.06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.10, 0.39, 0.48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.14, 0.40, 0.27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5, 0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add norm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5, 0.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.24, 1.18, 0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.76, 0.65, 0.27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repeat the training of 8_3 – 8_6 for longer iterations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.02, 0.32, 0.15</t>
   </si>
 </sst>
 </file>
@@ -7116,7 +7194,7 @@
   </sheetPr>
   <dimension ref="A1:N114"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
     </sheetView>
   </sheetViews>
@@ -8546,16 +8624,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q67"/>
+  <dimension ref="A1:Q82"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K68" activeCellId="0" sqref="K68"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P82" activeCellId="0" sqref="P82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="7" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.2834008097166"/>
     <col collapsed="false" hidden="false" max="14" min="9" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.3238866396761"/>
@@ -8952,11 +9030,11 @@
         <v>307</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>308</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>309</v>
       </c>
       <c r="F31" s="0" t="n">
@@ -8988,11 +9066,11 @@
         <v>302</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>313</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>314</v>
       </c>
     </row>
@@ -9132,7 +9210,7 @@
       <c r="A47" s="0" t="s">
         <v>327</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="C47" s="0" t="s">
         <v>328</v>
       </c>
       <c r="G47" s="0" t="n">
@@ -9168,7 +9246,7 @@
       <c r="A50" s="0" t="s">
         <v>333</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="C50" s="0" t="s">
         <v>334</v>
       </c>
       <c r="H50" s="0" t="s">
@@ -9182,7 +9260,7 @@
       <c r="A51" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="C51" s="0" t="s">
         <v>337</v>
       </c>
       <c r="H51" s="0" t="s">
@@ -9224,7 +9302,7 @@
       <c r="A54" s="0" t="s">
         <v>343</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="C54" s="0" t="s">
         <v>344</v>
       </c>
       <c r="H54" s="0" t="s">
@@ -9241,7 +9319,7 @@
       <c r="A56" s="0" t="s">
         <v>346</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="C56" s="0" t="s">
         <v>347</v>
       </c>
       <c r="G56" s="0" t="s">
@@ -9289,7 +9367,7 @@
       <c r="A60" s="0" t="s">
         <v>352</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="C60" s="0" t="s">
         <v>353</v>
       </c>
       <c r="G60" s="0" t="s">
@@ -9309,7 +9387,7 @@
       <c r="A62" s="0" t="s">
         <v>355</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="C62" s="0" t="s">
         <v>356</v>
       </c>
       <c r="G62" s="0" t="s">
@@ -9349,24 +9427,176 @@
       <c r="O65" s="0" t="n">
         <v>0.001</v>
       </c>
+      <c r="P65" s="0" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>360</v>
-      </c>
-      <c r="B66" s="0" t="s">
         <v>361</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>362</v>
       </c>
       <c r="O66" s="0" t="n">
         <v>0.005</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K67" s="0" t="n">
+      <c r="P66" s="0" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>365</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I69" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K69" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="O67" s="0" t="n">
+      <c r="O69" s="0" t="n">
         <v>0.001</v>
+      </c>
+      <c r="P69" s="0" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>367</v>
+      </c>
+      <c r="G70" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P70" s="0" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>369</v>
+      </c>
+      <c r="G71" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K71" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P71" s="0" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>371</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="K72" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="P72" s="0" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K73" s="0" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>374</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>375</v>
+      </c>
+      <c r="K74" s="0" t="s">
+        <v>376</v>
+      </c>
+      <c r="P74" s="0" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="P75" s="0" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>381</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>382</v>
+      </c>
+      <c r="F78" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="K78" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="K79" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="K80" s="0" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>385</v>
+      </c>
+      <c r="K81" s="0" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="K82" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="P82" s="0" t="s">
+        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extend unlabeled data UCF101, add coco labeled data
</commit_message>
<xml_diff>
--- a/exp_notes.xlsx
+++ b/exp_notes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="393">
   <si>
     <r>
       <rPr>
@@ -6949,6 +6949,21 @@
   </si>
   <si>
     <t xml:space="preserve">0.02, 0.32, 0.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8_13_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">more aug(10, 80, 80)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add UCF101 Unlabel(1484 seqs), COCO Label(680 imgs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aug(10,60,60)</t>
   </si>
 </sst>
 </file>
@@ -7202,7 +7217,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8178137651822"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
@@ -7212,7 +7227,7 @@
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="45.5263157894737"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="45.9554655870445"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8624,20 +8639,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q82"/>
+  <dimension ref="A1:Q88"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P82" activeCellId="0" sqref="P82"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L89" activeCellId="0" sqref="L89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="7" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.2834008097166"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.31983805668016"/>
     <col collapsed="false" hidden="false" max="14" min="9" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.3238866396761"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="48.417004048583"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="48.8461538461539"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -9597,6 +9612,43 @@
       </c>
       <c r="P82" s="0" t="s">
         <v>387</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>388</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>389</v>
+      </c>
+      <c r="F83" s="0" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>391</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>392</v>
+      </c>
+      <c r="K86" s="0" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K87" s="0" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K88" s="0" t="n">
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add normalization to the output of the model
</commit_message>
<xml_diff>
--- a/exp_notes.xlsx
+++ b/exp_notes.xlsx
@@ -21,15 +21,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="393">
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="397">
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">predictor</t>
     </r>
@@ -39,7 +38,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">实验记录</t>
     </r>
@@ -90,7 +88,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">训练</t>
     </r>
@@ -100,7 +97,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">encoder-decoder</t>
     </r>
@@ -112,7 +108,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">网络结构</t>
     </r>
@@ -122,7 +117,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">: [4,4,3,4,2]</t>
     </r>
@@ -137,7 +131,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">输入</t>
     </r>
@@ -147,7 +140,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">28x28</t>
     </r>
@@ -157,7 +149,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，压缩到</t>
     </r>
@@ -167,7 +158,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">32</t>
     </r>
@@ -179,7 +169,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">纯</t>
     </r>
@@ -189,7 +178,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">CNN</t>
     </r>
@@ -199,7 +187,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的</t>
     </r>
@@ -209,7 +196,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ED</t>
     </r>
@@ -227,7 +213,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5</t>
     </r>
@@ -237,7 +222,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">层</t>
     </r>
@@ -247,7 +231,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+5</t>
     </r>
@@ -257,7 +240,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">层</t>
     </r>
@@ -267,7 +249,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[1,8,16,16,32,32]</t>
     </r>
@@ -297,7 +278,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">全黑，试了各种</t>
     </r>
@@ -307,7 +287,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">lr</t>
     </r>
@@ -317,7 +296,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">和</t>
     </r>
@@ -327,7 +305,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">barch</t>
     </r>
@@ -337,7 +314,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -347,7 +323,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Adam</t>
     </r>
@@ -357,7 +332,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">和</t>
     </r>
@@ -367,7 +341,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">SGD</t>
     </r>
@@ -377,7 +350,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -387,7 +359,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">L1Loss</t>
     </r>
@@ -397,7 +368,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">一直保持</t>
     </r>
@@ -407,7 +377,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0.65</t>
     </r>
@@ -417,7 +386,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的</t>
     </r>
@@ -427,7 +395,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">loss</t>
     </r>
@@ -439,7 +406,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">warp</t>
     </r>
@@ -449,7 +415,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">后</t>
     </r>
@@ -459,7 +424,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">loss</t>
     </r>
@@ -469,7 +433,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">降了，但是</t>
     </r>
@@ -479,7 +442,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">tsne</t>
     </r>
@@ -489,7 +451,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">出来变差了</t>
     </r>
@@ -507,7 +468,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">与后面</t>
     </r>
@@ -517,7 +477,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">predict</t>
     </r>
@@ -527,7 +486,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">对比</t>
     </r>
@@ -545,7 +503,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">不是每次都能收敛</t>
     </r>
@@ -555,7 +512,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, </t>
     </r>
@@ -565,7 +521,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">测试</t>
     </r>
@@ -575,7 +530,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10000</t>
     </r>
@@ -585,7 +539,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步的还好，</t>
     </r>
@@ -595,7 +548,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">50000</t>
     </r>
@@ -605,7 +557,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步有很严重的</t>
     </r>
@@ -615,7 +566,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">overfitting</t>
     </r>
@@ -630,7 +580,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">warp</t>
     </r>
@@ -640,7 +589,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">改小</t>
     </r>
@@ -655,7 +603,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">也有</t>
     </r>
@@ -665,7 +612,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">overfitting</t>
     </r>
@@ -675,7 +621,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">。</t>
     </r>
@@ -685,7 +630,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1-4_10000.pkl</t>
     </r>
@@ -695,7 +639,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">后来被不小心覆盖了</t>
     </r>
@@ -707,7 +650,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">训练</t>
     </r>
@@ -717,7 +659,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">predictive</t>
     </r>
@@ -727,7 +668,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">网络</t>
     </r>
@@ -742,7 +682,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1_1_50000</t>
     </r>
@@ -752,7 +691,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">作为</t>
     </r>
@@ -762,7 +700,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ED</t>
     </r>
@@ -772,7 +709,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">模型</t>
     </r>
@@ -802,7 +738,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">bug loss</t>
     </r>
@@ -812,7 +747,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">图没存</t>
     </r>
@@ -842,7 +776,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">感觉预测挺准，但是</t>
     </r>
@@ -852,7 +785,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ED</t>
     </r>
@@ -862,7 +794,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">在</t>
     </r>
@@ -872,7 +803,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">warp</t>
     </r>
@@ -882,7 +812,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">数据上表现不好，画出来差点</t>
     </r>
@@ -900,7 +829,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2-5/6/7</t>
     </r>
@@ -910,7 +838,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">忘记改标号了，图和模型都没存</t>
     </r>
@@ -925,7 +852,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">改用</t>
     </r>
@@ -935,7 +861,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1_4_20000</t>
     </r>
@@ -945,7 +870,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">作为模型</t>
     </r>
@@ -963,7 +887,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">为什么大了一个数量级？？但是画出来结果还可以：输出</t>
     </r>
@@ -973,7 +896,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Encode</t>
     </r>
@@ -983,7 +905,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">层，</t>
     </r>
@@ -993,7 +914,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1_1</t>
     </r>
@@ -1003,7 +923,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的</t>
     </r>
@@ -1013,7 +932,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">std=1-2</t>
     </r>
@@ -1023,7 +941,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1033,7 +950,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1_4</t>
     </r>
@@ -1043,7 +959,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的</t>
     </r>
@@ -1053,7 +968,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">std=4-6</t>
     </r>
@@ -1065,7 +979,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">之前的实验中间那层没有</t>
     </r>
@@ -1075,7 +988,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Relu</t>
     </r>
@@ -1085,7 +997,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，看到有很大的负值，</t>
     </r>
@@ -1095,7 +1006,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">what if use Relu</t>
     </r>
@@ -1107,7 +1017,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">tsne</t>
     </r>
@@ -1117,7 +1026,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">出来比</t>
     </r>
@@ -1127,7 +1035,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1-4</t>
     </r>
@@ -1137,7 +1044,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">好太多，而且</t>
     </r>
@@ -1147,7 +1053,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">50000</t>
     </r>
@@ -1157,7 +1062,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步比</t>
     </r>
@@ -1167,7 +1071,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10000</t>
     </r>
@@ -1177,7 +1080,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步好太多，没有</t>
     </r>
@@ -1187,7 +1089,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1-3/1-4</t>
     </r>
@@ -1197,7 +1098,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">越迭代越差的现象，而且</t>
     </r>
@@ -1207,7 +1107,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">coding</t>
     </r>
@@ -1217,7 +1116,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的</t>
     </r>
@@ -1227,7 +1125,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">mean</t>
     </r>
@@ -1237,7 +1134,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">和</t>
     </r>
@@ -1247,7 +1143,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">var</t>
     </r>
@@ -1257,7 +1152,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">随着迭代减小（在并没有加入</t>
     </r>
@@ -1267,7 +1161,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">weight decay</t>
     </r>
@@ -1277,7 +1170,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的情况下），但是有</t>
     </r>
@@ -1287,7 +1179,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">dead relu</t>
     </r>
@@ -1297,7 +1188,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，不</t>
     </r>
@@ -1307,7 +1197,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">dead</t>
     </r>
@@ -1317,7 +1206,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的基本从来不是</t>
     </r>
@@ -1327,7 +1215,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0</t>
     </r>
@@ -1339,7 +1226,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3-x</t>
     </r>
@@ -1349,7 +1235,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">都</t>
     </r>
@@ -1359,7 +1244,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Train</t>
     </r>
@@ -1369,7 +1253,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">错了！！并没有用</t>
     </r>
@@ -1379,7 +1262,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">warp</t>
     </r>
@@ -1389,7 +1271,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">得图片</t>
     </r>
@@ -1407,7 +1288,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1-4</t>
     </r>
@@ -1417,7 +1297,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">基础上加上中间</t>
     </r>
@@ -1427,7 +1306,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Relu</t>
     </r>
@@ -1439,7 +1317,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">我想要稀疏的</t>
     </r>
@@ -1449,7 +1326,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">coding</t>
     </r>
@@ -1461,7 +1337,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[-0.1,0.1]</t>
     </r>
@@ -1471,7 +1346,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（并没</t>
     </r>
@@ -1481,7 +1355,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">warp</t>
     </r>
@@ -1491,7 +1364,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -1506,7 +1378,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">code</t>
     </r>
@@ -1516,7 +1387,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">数值很大（</t>
     </r>
@@ -1526,7 +1396,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10000</t>
     </r>
@@ -1536,7 +1405,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -1546,7 +1414,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mean=7</t>
     </r>
@@ -1556,7 +1423,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1566,7 +1432,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Std=4.6</t>
     </r>
@@ -1576,7 +1441,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1586,7 +1450,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">#0=5</t>
     </r>
@@ -1598,7 +1461,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5</t>
     </r>
@@ -1608,7 +1470,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">个</t>
     </r>
@@ -1618,7 +1479,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0</t>
     </r>
@@ -1628,7 +1488,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">是</t>
     </r>
@@ -1638,7 +1497,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">dead relu</t>
     </r>
@@ -1648,7 +1506,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -1658,7 +1515,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">30000</t>
     </r>
@@ -1668,7 +1524,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -1678,7 +1533,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mean=3</t>
     </r>
@@ -1688,7 +1542,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1698,7 +1551,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Std=2</t>
     </r>
@@ -1708,7 +1560,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1718,7 +1569,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">#0=5</t>
     </r>
@@ -1730,7 +1580,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5</t>
     </r>
@@ -1740,7 +1589,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">个</t>
     </r>
@@ -1750,7 +1598,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0</t>
     </r>
@@ -1760,7 +1607,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">是</t>
     </r>
@@ -1770,7 +1616,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">dead relu</t>
     </r>
@@ -1780,7 +1625,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -1790,7 +1634,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">50000</t>
     </r>
@@ -1800,7 +1643,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -1810,7 +1652,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mean=2</t>
     </r>
@@ -1820,7 +1661,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1830,7 +1670,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Std=1.3</t>
     </r>
@@ -1840,7 +1679,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1850,7 +1688,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">#0=5</t>
     </r>
@@ -1865,7 +1702,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">加</t>
     </r>
@@ -1875,7 +1711,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Regularization, weight_decay=1e-5</t>
     </r>
@@ -1887,7 +1722,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(10000</t>
     </r>
@@ -1897,7 +1731,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -1907,7 +1740,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mean=4.6</t>
     </r>
@@ -1917,7 +1749,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1927,7 +1758,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Std=4</t>
     </r>
@@ -1937,7 +1767,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -1947,7 +1776,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">#0=10</t>
     </r>
@@ -1959,7 +1787,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -1969,7 +1796,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">更多</t>
     </r>
@@ -1979,7 +1805,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">dead relu</t>
     </r>
@@ -1989,7 +1814,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，没有</t>
     </r>
@@ -1999,7 +1823,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3-1</t>
     </r>
@@ -2009,7 +1832,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">好</t>
     </r>
@@ -2019,7 +1841,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -2031,7 +1852,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -2041,7 +1861,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">30000</t>
     </r>
@@ -2051,7 +1870,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -2061,7 +1879,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mean=3.2</t>
     </r>
@@ -2071,7 +1888,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2081,7 +1897,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Std=2.8</t>
     </r>
@@ -2091,7 +1906,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2101,7 +1915,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">#0=10</t>
     </r>
@@ -2113,7 +1926,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -2123,7 +1935,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">50000</t>
     </r>
@@ -2133,7 +1944,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -2143,7 +1953,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mean=2.88</t>
     </r>
@@ -2153,7 +1962,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2163,7 +1971,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Std=2.5</t>
     </r>
@@ -2173,7 +1980,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2183,7 +1989,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">#0=9</t>
     </r>
@@ -2201,7 +2006,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(10000</t>
     </r>
@@ -2211,7 +2015,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -2221,7 +2024,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mean=6.25</t>
     </r>
@@ -2231,7 +2033,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2241,7 +2042,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Std=7.2</t>
     </r>
@@ -2251,7 +2051,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2261,7 +2060,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">#0=14</t>
     </r>
@@ -2273,7 +2071,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -2283,7 +2080,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">更多</t>
     </r>
@@ -2293,7 +2089,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">dead relu</t>
     </r>
@@ -2303,7 +2098,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，没有</t>
     </r>
@@ -2313,7 +2107,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3-2</t>
     </r>
@@ -2323,7 +2116,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">好</t>
     </r>
@@ -2333,7 +2125,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -2345,7 +2136,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -2355,7 +2145,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">30000</t>
     </r>
@@ -2365,7 +2154,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -2375,7 +2163,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mean=6.6</t>
     </r>
@@ -2385,7 +2172,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2395,7 +2181,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Std=7.5</t>
     </r>
@@ -2405,7 +2190,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2415,7 +2199,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">#0=14</t>
     </r>
@@ -2427,7 +2210,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -2437,7 +2219,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">50000</t>
     </r>
@@ -2447,7 +2228,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -2457,7 +2237,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mean=6.5</t>
     </r>
@@ -2467,7 +2246,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2477,7 +2255,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Std=7.3</t>
     </r>
@@ -2487,7 +2264,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2497,7 +2273,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">#0=14</t>
     </r>
@@ -2509,7 +2284,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">为什么没有那种有的时候是</t>
     </r>
@@ -2519,7 +2293,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0</t>
     </r>
@@ -2529,7 +2302,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">有的时候不是</t>
     </r>
@@ -2539,7 +2311,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0</t>
     </r>
@@ -2549,7 +2320,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的神经元？？（怎么得到稀疏的</t>
     </r>
@@ -2559,7 +2329,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">coding</t>
     </r>
@@ -2569,7 +2338,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -2584,7 +2352,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">在</t>
     </r>
@@ -2594,7 +2361,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3-2</t>
     </r>
@@ -2604,7 +2370,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">基础上，改</t>
     </r>
@@ -2614,7 +2379,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">LeakyReLU</t>
     </r>
@@ -2626,7 +2390,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(10000</t>
     </r>
@@ -2636,7 +2399,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -2646,7 +2408,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mean=5.4</t>
     </r>
@@ -2656,7 +2417,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2666,7 +2426,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Std=2.76</t>
     </r>
@@ -2676,7 +2435,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2686,7 +2444,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">#0=0.26</t>
     </r>
@@ -2701,7 +2458,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -2711,7 +2467,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">30000</t>
     </r>
@@ -2721,7 +2476,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -2731,7 +2485,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mean=3.9</t>
     </r>
@@ -2741,7 +2494,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2751,7 +2503,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Std=1.9</t>
     </r>
@@ -2761,7 +2512,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2771,7 +2521,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">#0=0.23</t>
     </r>
@@ -2783,7 +2532,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -2793,7 +2541,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">50000</t>
     </r>
@@ -2803,7 +2550,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -2813,7 +2559,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Mean=3.6</t>
     </r>
@@ -2823,7 +2568,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2833,7 +2577,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Std=1.75</t>
     </r>
@@ -2843,7 +2586,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -2853,7 +2595,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">#0=0.2</t>
     </r>
@@ -2865,7 +2606,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">因为</t>
     </r>
@@ -2875,7 +2615,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3-x</t>
     </r>
@@ -2885,7 +2624,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">没</t>
     </r>
@@ -2895,7 +2633,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">warp</t>
     </r>
@@ -2910,7 +2647,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3_1_50000</t>
     </r>
@@ -2920,7 +2656,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">作为</t>
     </r>
@@ -2930,7 +2665,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ED</t>
     </r>
@@ -2940,7 +2674,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">模型</t>
     </r>
@@ -2952,7 +2685,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">预测得挺好，但是</t>
     </r>
@@ -2962,7 +2694,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">decoder</t>
     </r>
@@ -2972,7 +2703,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">不好，</t>
     </r>
@@ -2982,7 +2712,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">decode</t>
     </r>
@@ -2992,7 +2721,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">出来的变类别，比如</t>
     </r>
@@ -3002,7 +2730,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -3012,7 +2739,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">变</t>
     </r>
@@ -3022,7 +2748,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">9</t>
     </r>
@@ -3032,7 +2757,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -3042,7 +2766,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -3052,7 +2775,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">变</t>
     </r>
@@ -3062,7 +2784,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
     </r>
@@ -3072,7 +2793,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">之类</t>
     </r>
@@ -3087,7 +2807,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">修正</t>
     </r>
@@ -3097,7 +2816,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3-x</t>
     </r>
@@ -3107,7 +2825,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的</t>
     </r>
@@ -3117,7 +2834,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">warp</t>
     </r>
@@ -3127,7 +2843,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">问题重新来（</t>
     </r>
@@ -3137,7 +2852,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">weight_decay=1e-5</t>
     </r>
@@ -3147,7 +2861,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">）</t>
     </r>
@@ -3162,7 +2875,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（</t>
     </r>
@@ -3172,7 +2884,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ED</t>
     </r>
@@ -3182,7 +2893,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">得可以，但是</t>
     </r>
@@ -3192,7 +2902,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">tsne</t>
     </r>
@@ -3202,7 +2911,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">不好，</t>
     </r>
@@ -3212,7 +2920,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -3222,7 +2929,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">和</t>
     </r>
@@ -3232,7 +2938,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">9</t>
     </r>
@@ -3242,7 +2947,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">特别近）</t>
     </r>
@@ -3263,7 +2967,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">去掉忘记去掉得</t>
     </r>
@@ -3273,7 +2976,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">weight_decay</t>
     </r>
@@ -3297,7 +2999,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5_1_50000</t>
     </r>
@@ -3307,7 +3008,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">作为</t>
     </r>
@@ -3317,7 +3017,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ED</t>
     </r>
@@ -3327,7 +3026,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">模型</t>
     </r>
@@ -3339,7 +3037,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">还是会变类别，特别是</t>
     </r>
@@ -3349,7 +3046,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -3359,7 +3055,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">和</t>
     </r>
@@ -3369,7 +3064,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">9</t>
     </r>
@@ -3381,7 +3075,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">震惊！！我从</t>
     </r>
@@ -3391,7 +3084,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1-3</t>
     </r>
@@ -3401,7 +3093,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">起，</t>
     </r>
@@ -3411,7 +3102,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ED</t>
     </r>
@@ -3421,7 +3111,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">一直用得是</t>
     </r>
@@ -3431,7 +3120,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">SmoothL1</t>
     </r>
@@ -3441,7 +3129,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">！！！我记得不是不行嘛。。。</t>
     </r>
@@ -3453,7 +3140,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">由于我的输出值基本上是</t>
     </r>
@@ -3463,7 +3149,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0-1</t>
     </r>
@@ -3473,7 +3158,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">之间得，因此</t>
     </r>
@@ -3483,7 +3167,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">SmoothL1</t>
     </r>
@@ -3493,7 +3176,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">就相当于</t>
     </r>
@@ -3503,7 +3185,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">L2</t>
     </r>
@@ -3513,7 +3194,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">！！</t>
     </r>
@@ -3552,7 +3232,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">改用</t>
     </r>
@@ -3562,7 +3241,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">adam</t>
     </r>
@@ -3572,7 +3250,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，很容易收敛</t>
     </r>
@@ -3587,7 +3264,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5</t>
     </r>
@@ -3597,7 +3273,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">层</t>
     </r>
@@ -3607,7 +3282,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">+5</t>
     </r>
@@ -3617,7 +3291,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">层</t>
     </r>
@@ -3627,7 +3300,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[16,32,64,128,256]</t>
     </r>
@@ -3639,7 +3311,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">地图减小，输入减小到</t>
     </r>
@@ -3649,7 +3320,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">65x65</t>
     </r>
@@ -3664,7 +3334,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">训练</t>
     </r>
@@ -3674,7 +3343,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">predictor</t>
     </r>
@@ -3684,7 +3352,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -3694,7 +3361,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">batch=1</t>
     </r>
@@ -3704,7 +3370,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">不行，刚开始</t>
     </r>
@@ -3714,7 +3379,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">action</t>
     </r>
@@ -3724,7 +3388,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">用</t>
     </r>
@@ -3734,7 +3397,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -3744,7 +3406,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">个</t>
     </r>
@@ -3754,7 +3415,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0-1</t>
     </r>
@@ -3764,7 +3424,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的向量表示，后来简化到</t>
     </r>
@@ -3774,7 +3433,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">one-hot</t>
     </r>
@@ -3786,7 +3444,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">输入</t>
     </r>
@@ -3796,7 +3453,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">encode</t>
     </r>
@@ -3806,7 +3462,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">和</t>
     </r>
@@ -3816,7 +3471,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">action</t>
     </r>
@@ -3826,7 +3480,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，预测下一个</t>
     </r>
@@ -3836,7 +3489,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">encode</t>
     </r>
@@ -3851,7 +3503,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">单隐层</t>
     </r>
@@ -3861,7 +3512,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">512</t>
     </r>
@@ -3873,7 +3523,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">130000</t>
     </r>
@@ -3883,7 +3532,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，每</t>
     </r>
@@ -3893,7 +3541,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">50000</t>
     </r>
@@ -3903,7 +3550,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">降</t>
     </r>
@@ -3913,7 +3559,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0.2</t>
     </r>
@@ -3925,7 +3570,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">有</t>
     </r>
@@ -3935,7 +3579,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">loss</t>
     </r>
@@ -3945,7 +3588,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">图</t>
     </r>
@@ -3960,7 +3602,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">双隐层</t>
     </r>
@@ -3970,7 +3611,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[512,512]</t>
     </r>
@@ -3982,7 +3622,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">有</t>
     </r>
@@ -3992,7 +3631,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">loss</t>
     </r>
@@ -4002,7 +3640,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">图</t>
     </r>
@@ -4012,7 +3649,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">, </t>
     </r>
@@ -4022,7 +3658,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">有</t>
     </r>
@@ -4032,7 +3667,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">test</t>
     </r>
@@ -4042,7 +3676,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">图，要训练这么多步才能记下一张地图</t>
     </r>
@@ -4054,7 +3687,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">共同训练</t>
     </r>
@@ -4064,7 +3696,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">encoder-decoder</t>
     </r>
@@ -4074,7 +3705,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">和</t>
     </r>
@@ -4084,7 +3714,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">predictor</t>
     </r>
@@ -4094,7 +3723,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，期待</t>
     </r>
@@ -4104,7 +3732,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">predictor</t>
     </r>
@@ -4114,7 +3741,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">能成为一个</t>
     </r>
@@ -4124,7 +3750,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">regularizer</t>
     </r>
@@ -4134,7 +3759,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，使得</t>
     </r>
@@ -4144,7 +3768,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">encoder</t>
     </r>
@@ -4154,7 +3777,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">出来的更像</t>
     </r>
@@ -4164,7 +3786,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">toponode</t>
     </r>
@@ -4176,7 +3797,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">用</t>
     </r>
@@ -4186,7 +3806,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
     </r>
@@ -4196,7 +3815,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">和</t>
     </r>
@@ -4206,7 +3824,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2.2</t>
     </r>
@@ -4216,7 +3833,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">中</t>
     </r>
@@ -4226,7 +3842,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">train</t>
     </r>
@@ -4236,7 +3851,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">好的模型再一起</t>
     </r>
@@ -4246,7 +3860,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">finetune</t>
     </r>
@@ -4258,7 +3871,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">每个</t>
     </r>
@@ -4268,7 +3880,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">step</t>
     </r>
@@ -4278,7 +3889,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -4288,7 +3898,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ED(encode/decode)</t>
     </r>
@@ -4298,7 +3907,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">和</t>
     </r>
@@ -4308,7 +3916,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Pred(pred/encode)</t>
     </r>
@@ -4318,7 +3925,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">要分开更新，</t>
     </r>
@@ -4328,7 +3934,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">encode</t>
     </r>
@@ -4338,7 +3943,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">在两个地方更新不能用</t>
     </r>
@@ -4348,7 +3952,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">momentum</t>
     </r>
@@ -4358,7 +3961,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -4368,7 +3970,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5</t>
     </r>
@@ -4378,7 +3979,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">个参数</t>
     </r>
@@ -4388,7 +3988,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">lr_pred, lr_state, lr_state_when_pred, pred_num, ed_num</t>
     </r>
@@ -4403,7 +4002,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">train</t>
     </r>
@@ -4413,7 +4011,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">好的</t>
     </r>
@@ -4423,7 +4020,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ED</t>
     </r>
@@ -4433,7 +4029,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，</t>
     </r>
@@ -4443,7 +4038,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">pred</t>
     </r>
@@ -4458,7 +4052,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.05,0.0001] 30000</t>
     </r>
@@ -4468,7 +4061,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -4478,7 +4070,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4ED-1Pred</t>
     </r>
@@ -4493,7 +4084,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">不是每次都能收敛，训练不稳定，有</t>
     </r>
@@ -4503,7 +4093,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">loss</t>
     </r>
@@ -4513,7 +4102,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">图</t>
     </r>
@@ -4525,7 +4113,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">慢慢加大</t>
     </r>
@@ -4535,7 +4122,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">speed[40,70,100,130,170,230]</t>
     </r>
@@ -4547,7 +4133,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">之前</t>
     </r>
@@ -4557,7 +4142,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">speed</t>
     </r>
@@ -4567,7 +4151,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">太小，猜想</t>
     </r>
@@ -4577,7 +4160,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">regularize</t>
     </r>
@@ -4587,7 +4169,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">不动</t>
     </r>
@@ -4605,7 +4186,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.05,0.0005] 10000</t>
     </r>
@@ -4615,7 +4195,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -4625,7 +4204,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">20ED-10Pred</t>
     </r>
@@ -4637,7 +4215,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ed</t>
     </r>
@@ -4647,7 +4224,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">一直在降，</t>
     </r>
@@ -4657,7 +4233,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">pred</t>
     </r>
@@ -4667,7 +4242,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">变差，速度大时</t>
     </r>
@@ -4677,7 +4251,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">pred</t>
     </r>
@@ -4687,7 +4260,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">全白图</t>
     </r>
@@ -4699,7 +4271,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ed</t>
     </r>
@@ -4709,7 +4280,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的结果更清晰了，但是没有被</t>
     </r>
@@ -4719,7 +4289,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">regularize</t>
     </r>
@@ -4729,7 +4298,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的效果</t>
     </r>
@@ -4741,7 +4309,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">加大</t>
     </r>
@@ -4751,7 +4318,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">pred</t>
     </r>
@@ -4761,7 +4327,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的</t>
     </r>
@@ -4771,7 +4336,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">lr</t>
     </r>
@@ -4781,7 +4345,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">和更新比例</t>
     </r>
@@ -4793,7 +4356,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3.3</t>
     </r>
@@ -4803,7 +4365,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的</t>
     </r>
@@ -4813,7 +4374,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">speed=170</t>
     </r>
@@ -4825,7 +4385,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.05,0.001] 10000</t>
     </r>
@@ -4835,7 +4394,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -4845,7 +4403,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">20ED-20Pred</t>
     </r>
@@ -4860,7 +4417,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.01,0.05,0.01] 10000</t>
     </r>
@@ -4870,7 +4426,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -4880,7 +4435,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">20ED-20Pred</t>
     </r>
@@ -4895,7 +4449,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">实验</t>
     </r>
@@ -4905,7 +4458,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -4915,7 +4467,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">都做错了，</t>
     </r>
@@ -4925,7 +4476,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">predictor</t>
     </r>
@@ -4935,7 +4485,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">都没有</t>
     </r>
@@ -4945,7 +4494,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">relu</t>
     </r>
@@ -4957,7 +4505,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">从</t>
     </r>
@@ -4967,7 +4514,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">scratch</t>
     </r>
@@ -4977,7 +4523,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">开始</t>
     </r>
@@ -4987,7 +4532,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">train</t>
     </r>
@@ -4997,7 +4541,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">起</t>
     </r>
@@ -5012,7 +4555,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.0001,0.001,0.0001] 10000</t>
     </r>
@@ -5022,7 +4564,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5032,7 +4573,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10ED-10Pred</t>
     </r>
@@ -5044,7 +4584,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.009,20] pred</t>
     </r>
@@ -5054,7 +4593,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">弱</t>
     </r>
@@ -5066,7 +4604,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">encoder</t>
     </r>
@@ -5076,7 +4613,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">参数分开两个</t>
     </r>
@@ -5086,7 +4622,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">adam</t>
     </r>
@@ -5101,7 +4636,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 10000</t>
     </r>
@@ -5111,7 +4645,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5121,7 +4654,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10ED-10Pred</t>
     </r>
@@ -5133,7 +4665,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.026,0] ed</t>
     </r>
@@ -5143,7 +4674,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">弱</t>
     </r>
@@ -5158,7 +4688,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 10000</t>
     </r>
@@ -5168,7 +4697,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5178,7 +4706,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10ED-5Pred</t>
     </r>
@@ -5190,7 +4717,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.024,0] ed</t>
     </r>
@@ -5200,7 +4726,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">弱</t>
     </r>
@@ -5215,7 +4740,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 10000</t>
     </r>
@@ -5225,7 +4749,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5235,7 +4758,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10ED-2Pred</t>
     </r>
@@ -5247,7 +4769,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.0067,2.1] pred</t>
     </r>
@@ -5257,7 +4778,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">弱</t>
     </r>
@@ -5272,7 +4792,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 10000</t>
     </r>
@@ -5282,7 +4801,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5292,7 +4810,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10ED-3Pred</t>
     </r>
@@ -5304,7 +4821,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.0067,0.4] </t>
     </r>
@@ -5314,7 +4830,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">正好</t>
     </r>
@@ -5329,7 +4844,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.0085,0.7] </t>
     </r>
@@ -5339,7 +4853,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">还好</t>
     </r>
@@ -5354,7 +4867,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 10000</t>
     </r>
@@ -5364,7 +4876,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5374,7 +4885,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10ED-20Pred</t>
     </r>
@@ -5389,7 +4899,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 10000</t>
     </r>
@@ -5399,7 +4908,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5409,7 +4917,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10ED-15Pred</t>
     </r>
@@ -5421,7 +4928,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.01,0.1] </t>
     </r>
@@ -5431,7 +4937,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">？？</t>
     </r>
@@ -5446,7 +4951,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">单隐层</t>
     </r>
@@ -5456,7 +4960,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">256</t>
     </r>
@@ -5477,7 +4980,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">单隐层</t>
     </r>
@@ -5487,7 +4989,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">64</t>
     </r>
@@ -5505,7 +5006,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 10000</t>
     </r>
@@ -5515,7 +5015,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5525,7 +5024,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3ED-10Pred</t>
     </r>
@@ -5537,7 +5035,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.0096,0.19] pred</t>
     </r>
@@ -5547,7 +5044,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">弱</t>
     </r>
@@ -5557,7 +5053,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">(</t>
     </r>
@@ -5567,7 +5062,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">白</t>
     </r>
@@ -5577,7 +5071,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">)</t>
     </r>
@@ -5595,7 +5088,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 10000</t>
     </r>
@@ -5605,7 +5097,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5615,7 +5106,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3ED-7Pred</t>
     </r>
@@ -5627,7 +5117,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.013,1000+] pred</t>
     </r>
@@ -5637,7 +5126,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">弱</t>
     </r>
@@ -5655,7 +5143,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 10000</t>
     </r>
@@ -5665,7 +5152,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5675,7 +5161,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1ED-2Pred</t>
     </r>
@@ -5687,7 +5172,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.02,1000+] pred</t>
     </r>
@@ -5697,7 +5181,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">弱</t>
     </r>
@@ -5715,7 +5198,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 10000</t>
     </r>
@@ -5725,7 +5207,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5735,7 +5216,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2ED-5Pred</t>
     </r>
@@ -5753,7 +5233,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 20000</t>
     </r>
@@ -5763,7 +5242,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5773,7 +5251,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2ED-10Pred</t>
     </r>
@@ -5785,7 +5262,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.009,2.5] </t>
     </r>
@@ -5795,7 +5271,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">超好</t>
     </r>
@@ -5810,7 +5285,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 20000</t>
     </r>
@@ -5820,7 +5294,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5830,7 +5303,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3ED-10Pred</t>
     </r>
@@ -5848,7 +5320,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 20000</t>
     </r>
@@ -5858,7 +5329,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5868,7 +5338,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3ED-7Pred</t>
     </r>
@@ -5886,7 +5355,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 20000</t>
     </r>
@@ -5896,7 +5364,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5906,7 +5373,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1ED-2Pred</t>
     </r>
@@ -5924,7 +5390,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 20000</t>
     </r>
@@ -5934,7 +5399,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5944,7 +5408,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2ED-5Pred</t>
     </r>
@@ -5956,7 +5419,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.008,1] pred</t>
     </r>
@@ -5966,7 +5428,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">不好</t>
     </r>
@@ -5978,7 +5439,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 20000</t>
     </r>
@@ -5988,7 +5448,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -5998,7 +5457,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1ED-10Pred</t>
     </r>
@@ -6013,7 +5471,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.0001,0.001,0.0001] 20000</t>
     </r>
@@ -6023,7 +5480,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -6033,7 +5489,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1ED-10Pred</t>
     </r>
@@ -6048,7 +5503,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.0001,0.001,0.0001] 20000</t>
     </r>
@@ -6058,7 +5512,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -6068,7 +5521,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1ED-20Pred</t>
     </r>
@@ -6083,7 +5535,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.0001,0.0001,0.0001] 20000</t>
     </r>
@@ -6093,7 +5544,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -6103,7 +5553,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1ED-5Pred</t>
     </r>
@@ -6121,7 +5570,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 20000</t>
     </r>
@@ -6131,7 +5579,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -6141,7 +5588,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">10ED-3Pred</t>
     </r>
@@ -6153,7 +5599,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.0056,0.2]</t>
     </r>
@@ -6163,7 +5608,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">预测和</t>
     </r>
@@ -6173,7 +5617,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">encode</t>
     </r>
@@ -6183,7 +5626,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">完美但</t>
     </r>
@@ -6193,7 +5635,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">predictor</t>
     </r>
@@ -6203,7 +5644,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">的</t>
     </r>
@@ -6213,7 +5653,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">regulate</t>
     </r>
@@ -6223,7 +5662,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">作用弱</t>
     </r>
@@ -6238,7 +5676,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.008,0.004]</t>
     </r>
@@ -6248,7 +5685,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">更完美</t>
     </r>
@@ -6263,7 +5699,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.009,0.004]predictor</t>
     </r>
@@ -6273,7 +5708,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">强了怎样都行</t>
     </r>
@@ -6288,7 +5722,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 20000</t>
     </r>
@@ -6298,7 +5731,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -6308,7 +5740,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1ED-5Pred</t>
     </r>
@@ -6320,7 +5751,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.024,0]ed</t>
     </r>
@@ -6330,7 +5760,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">弱</t>
     </r>
@@ -6348,7 +5777,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3lr=[0.001,0.001,0.001] 20000</t>
     </r>
@@ -6358,7 +5786,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步，</t>
     </r>
@@ -6368,7 +5795,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1ED-3Pred</t>
     </r>
@@ -6383,7 +5809,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">接</t>
     </r>
@@ -6393,7 +5818,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5_1</t>
     </r>
@@ -6403,7 +5827,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">训练</t>
     </r>
@@ -6413,7 +5836,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2000</t>
     </r>
@@ -6423,7 +5845,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">步</t>
     </r>
@@ -6435,7 +5856,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">[0.008,0.035] </t>
     </r>
@@ -6445,7 +5865,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">超好</t>
     </r>
@@ -6550,7 +5969,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">随便试了各种参数，都不</t>
     </r>
@@ -6560,7 +5978,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">work</t>
     </r>
@@ -6662,7 +6079,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">换成</t>
     </r>
@@ -6672,7 +6088,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">regulariaze</t>
     </r>
@@ -6682,7 +6097,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">长度平方</t>
     </r>
@@ -6692,7 +6106,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">x0.1</t>
     </r>
@@ -6716,7 +6129,6 @@
         <color rgb="FF000000"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">改</t>
     </r>
@@ -6726,7 +6138,6 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">norm</t>
     </r>
@@ -6964,6 +6375,18 @@
   </si>
   <si>
     <t xml:space="preserve">Aug(10,60,60)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add normalization to the model to avoid small output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10_1</t>
   </si>
 </sst>
 </file>
@@ -6982,7 +6405,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -7004,7 +6426,6 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -7217,7 +6638,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
@@ -7227,7 +6648,7 @@
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="45.9554655870445"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="46.3805668016194"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8639,10 +8060,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q88"/>
+  <dimension ref="A1:Q92"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L89" activeCellId="0" sqref="L89"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H91" activeCellId="0" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -8651,8 +8072,8 @@
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.31983805668016"/>
     <col collapsed="false" hidden="false" max="14" min="9" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="48.8461538461539"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="49.2753036437247"/>
     <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -9642,13 +9063,40 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>393</v>
+      </c>
       <c r="K87" s="0" t="n">
         <v>0.1</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>394</v>
+      </c>
       <c r="K88" s="0" t="n">
         <v>0.02</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="G91" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K91" s="0" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K92" s="0" t="n">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small change for tracking dataset
</commit_message>
<xml_diff>
--- a/exp_notes.xlsx
+++ b/exp_notes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="438">
   <si>
     <r>
       <rPr>
@@ -6387,6 +6387,129 @@
   </si>
   <si>
     <t xml:space="preserve">10_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supervised</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.07, 0.56, 1.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.12, 0.61, 0.85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.19, 0.46, 0.64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supervised-pretrain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04, 0.49, 0.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">supervised pretrain help a little</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10_4_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb_21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continue 10_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10_5_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continue 10_2 with lam=0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add more labeled data, from 10_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.12, 0.53, 1.62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.34, 0.53, 0.71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.10, 0.50, 1.88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.07, 0.48, 1.26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.04, 0.50, 0.62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.18, 0.57, 1.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.11, 0.57, 0.95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.28, 0.66, 0.91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.17, 0.59, 0.60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.33, 0.76, 0.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.28, 0.72, 0.28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rescale augmentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12_4</t>
   </si>
 </sst>
 </file>
@@ -6630,7 +6753,7 @@
   </sheetPr>
   <dimension ref="A1:N114"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A59" activeCellId="0" sqref="A59"/>
     </sheetView>
   </sheetViews>
@@ -8060,10 +8183,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q92"/>
+  <dimension ref="A1:R119"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A59" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H91" activeCellId="0" sqref="H91"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L120" activeCellId="0" sqref="L120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -9087,16 +9210,317 @@
       <c r="A91" s="0" t="s">
         <v>396</v>
       </c>
+      <c r="B91" s="0" t="s">
+        <v>397</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="F91" s="0" t="n">
+        <v>10000</v>
+      </c>
       <c r="G91" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K91" s="0" t="n">
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>399</v>
+      </c>
+      <c r="F92" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="G92" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="K92" s="0" t="n">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K92" s="0" t="n">
+      <c r="O92" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="P92" s="0" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>401</v>
+      </c>
+      <c r="K93" s="0" t="n">
         <v>0.05</v>
+      </c>
+      <c r="O93" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="P93" s="0" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>403</v>
+      </c>
+      <c r="K94" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="O94" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="P94" s="0" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>405</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>406</v>
+      </c>
+      <c r="K95" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="O95" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="P95" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="Q95" s="0" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>409</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="F97" s="0" t="n">
+        <v>20000</v>
+      </c>
+      <c r="K97" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="O97" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="F98" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="K98" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O98" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>414</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>415</v>
+      </c>
+      <c r="F100" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="K100" s="0" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="O100" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="P100" s="0" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>417</v>
+      </c>
+      <c r="F101" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="K101" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="O101" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="P101" s="0" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>419</v>
+      </c>
+      <c r="K103" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="O103" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="P103" s="0" t="s">
+        <v>420</v>
+      </c>
+      <c r="Q103" s="0" t="s">
+        <v>421</v>
+      </c>
+      <c r="R103" s="0" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>423</v>
+      </c>
+      <c r="K104" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="O104" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="P104" s="0" t="s">
+        <v>424</v>
+      </c>
+      <c r="Q104" s="0" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>426</v>
+      </c>
+      <c r="K105" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="O105" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="P105" s="0" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q105" s="0" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="K106" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="O106" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="P106" s="0" t="s">
+        <v>430</v>
+      </c>
+      <c r="Q106" s="0" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="G109" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="K109" s="0" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="G113" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="K113" s="0" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="O113" s="0" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>435</v>
+      </c>
+      <c r="K114" s="0" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="O114" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>436</v>
+      </c>
+      <c r="K115" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="O115" s="0" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>437</v>
+      </c>
+      <c r="K116" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="O116" s="0" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K117" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="O117" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K118" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="O118" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K119" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="O119" s="0" t="n">
+        <v>0.0001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add duke dataset and do more exps
</commit_message>
<xml_diff>
--- a/exp_notes.xlsx
+++ b/exp_notes.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="496">
   <si>
     <r>
       <rPr>
@@ -6600,6 +6600,220 @@
   </si>
   <si>
     <t xml:space="preserve">21_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">train on a lot of car data using resnet18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIRAT, Koper, TITS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last 3 convs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.37,0.41, 0.45, 0.51(2000-10000-20000-30000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last 9 convs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.47, 0.46, 0.46, 0.50, 0.35(2000-10000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last 7 convs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">small conv net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">效果很差</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">先</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">一下再</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">train</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">32_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32_2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">在</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">基础上</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">train</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，并没有帮助</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">32_3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">加</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ATVtrain</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">41_1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">加</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">3DPES</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">41_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41_4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">加</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">DukeMTMC</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">41_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bao</t>
   </si>
 </sst>
 </file>
@@ -6851,7 +7065,7 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="6.85425101214575"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.497975708502"/>
@@ -6861,7 +7075,7 @@
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.53441295546559"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="46.3805668016194"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="47.0242914979757"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8273,31 +8487,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R146"/>
+  <dimension ref="A1:S168"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K146" activeCellId="0" sqref="K146"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A139" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R168" activeCellId="0" sqref="R168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.31983805668016"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="49.2753036437247"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="8" min="1" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.31983805668016"/>
+    <col collapsed="false" hidden="false" max="15" min="10" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.6032388663968"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="49.919028340081"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>248</v>
       </c>
     </row>
@@ -8305,52 +8520,53 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="M2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="N2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="O2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="P2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -8358,22 +8574,22 @@
       <c r="A3" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="M3" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="N3" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="O3" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="P3" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="Q3" s="0" t="n">
         <v>0.0022</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="R3" s="0" t="s">
         <v>257</v>
       </c>
     </row>
@@ -8381,10 +8597,10 @@
       <c r="A4" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="O4" s="0" t="n">
+      <c r="P4" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="P4" s="0" t="n">
+      <c r="Q4" s="0" t="n">
         <v>0.0014</v>
       </c>
     </row>
@@ -8392,28 +8608,28 @@
       <c r="A6" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="L6" s="0" t="s">
+      <c r="M6" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="N6" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="O6" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="O6" s="0" t="n">
+      <c r="P6" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="P6" s="0" t="n">
+      <c r="Q6" s="0" t="n">
         <v>2E-005</v>
       </c>
     </row>
@@ -8421,10 +8637,10 @@
       <c r="A7" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="R7" s="0" t="s">
         <v>266</v>
       </c>
     </row>
@@ -8432,7 +8648,7 @@
       <c r="A8" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="O8" s="0" t="n">
+      <c r="P8" s="0" t="n">
         <v>0.0001</v>
       </c>
     </row>
@@ -8440,10 +8656,10 @@
       <c r="A9" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="O9" s="0" t="n">
+      <c r="P9" s="0" t="n">
         <v>0.001</v>
       </c>
     </row>
@@ -8451,7 +8667,7 @@
       <c r="A10" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="O10" s="0" t="n">
+      <c r="P10" s="0" t="n">
         <v>0.0001</v>
       </c>
     </row>
@@ -8459,13 +8675,13 @@
       <c r="A11" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="O11" s="0" t="n">
+      <c r="P11" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="P11" s="0" t="s">
+      <c r="Q11" s="0" t="s">
         <v>273</v>
       </c>
     </row>
@@ -8473,10 +8689,10 @@
       <c r="A12" s="0" t="s">
         <v>274</v>
       </c>
-      <c r="O12" s="0" t="n">
+      <c r="P12" s="0" t="n">
         <v>0.0001</v>
       </c>
-      <c r="P12" s="0" t="s">
+      <c r="Q12" s="0" t="s">
         <v>275</v>
       </c>
     </row>
@@ -8484,10 +8700,10 @@
       <c r="A14" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="C14" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>278</v>
       </c>
     </row>
@@ -8520,22 +8736,22 @@
       <c r="A21" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="C21" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="D21" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="L21" s="0" t="s">
+      <c r="M21" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="M21" s="0" t="s">
+      <c r="N21" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="N21" s="0" t="n">
+      <c r="O21" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="O21" s="0" t="n">
+      <c r="P21" s="0" t="n">
         <v>0.001</v>
       </c>
     </row>
@@ -8543,10 +8759,10 @@
       <c r="A22" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="O22" s="0" t="n">
+      <c r="P22" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="P22" s="0" t="s">
+      <c r="Q22" s="0" t="s">
         <v>287</v>
       </c>
     </row>
@@ -8554,16 +8770,16 @@
       <c r="A24" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="L24" s="0" t="s">
+      <c r="M24" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="N24" s="0" t="n">
+      <c r="O24" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="O24" s="0" t="n">
+      <c r="P24" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="P24" s="0" t="s">
+      <c r="Q24" s="0" t="s">
         <v>290</v>
       </c>
     </row>
@@ -8571,28 +8787,28 @@
       <c r="A25" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="G25" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="H25" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H25" s="0" t="s">
+      <c r="I25" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="K25" s="0" t="n">
+      <c r="L25" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="N25" s="0" t="n">
+      <c r="O25" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="O25" s="0" t="n">
+      <c r="P25" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="P25" s="0" t="s">
+      <c r="Q25" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="Q25" s="0" t="s">
+      <c r="R25" s="0" t="s">
         <v>294</v>
       </c>
     </row>
@@ -8600,13 +8816,13 @@
       <c r="A26" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="G26" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="H26" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H26" s="0" t="s">
+      <c r="I26" s="0" t="s">
         <v>292</v>
       </c>
     </row>
@@ -8614,28 +8830,28 @@
       <c r="A28" s="0" t="s">
         <v>296</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="G28" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="G28" s="0" t="n">
+      <c r="H28" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="H28" s="0" t="s">
+      <c r="I28" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="I28" s="0" t="n">
+      <c r="J28" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="J28" s="0" t="n">
+      <c r="K28" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="L28" s="0" t="s">
+      <c r="M28" s="0" t="s">
         <v>298</v>
       </c>
-      <c r="O28" s="0" t="s">
+      <c r="P28" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="P28" s="0" t="s">
+      <c r="Q28" s="0" t="s">
         <v>300</v>
       </c>
     </row>
@@ -8643,19 +8859,19 @@
       <c r="A29" s="0" t="s">
         <v>301</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="G29" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="H29" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="H29" s="0" t="s">
+      <c r="I29" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="O29" s="0" t="s">
+      <c r="P29" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="P29" s="0" t="s">
+      <c r="Q29" s="0" t="s">
         <v>303</v>
       </c>
     </row>
@@ -8663,36 +8879,36 @@
       <c r="A30" s="0" t="s">
         <v>304</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="G30" s="0" t="n">
         <v>20000</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="H30" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="H30" s="0" t="s">
+      <c r="I30" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="O30" s="0" t="s">
+      <c r="P30" s="0" t="s">
         <v>306</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="R30" s="1" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>308</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="G31" s="0" t="n">
         <v>20000</v>
       </c>
-      <c r="H31" s="0" t="s">
+      <c r="I31" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="O31" s="0" t="s">
+      <c r="P31" s="0" t="s">
         <v>306</v>
       </c>
     </row>
@@ -8700,7 +8916,7 @@
       <c r="A32" s="0" t="s">
         <v>311</v>
       </c>
-      <c r="O32" s="0" t="s">
+      <c r="P32" s="0" t="s">
         <v>302</v>
       </c>
     </row>
@@ -8708,18 +8924,18 @@
       <c r="A33" s="0" t="s">
         <v>312</v>
       </c>
-      <c r="G33" s="0" t="n">
+      <c r="H33" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="O33" s="0" t="s">
+      <c r="P33" s="0" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="18.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>313</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>314</v>
       </c>
     </row>
@@ -8727,7 +8943,7 @@
       <c r="A36" s="0" t="s">
         <v>315</v>
       </c>
-      <c r="O36" s="0" t="n">
+      <c r="P36" s="0" t="n">
         <v>0.001</v>
       </c>
     </row>
@@ -8735,32 +8951,32 @@
       <c r="A37" s="0" t="s">
         <v>316</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="G37" s="0" t="n">
         <v>2000</v>
       </c>
-      <c r="G37" s="0" t="n">
+      <c r="H37" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="H37" s="0" t="s">
+      <c r="I37" s="0" t="s">
         <v>292</v>
       </c>
-      <c r="O37" s="0" t="n">
+      <c r="P37" s="0" t="n">
         <v>0.001</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F38" s="0" t="n">
+      <c r="G38" s="0" t="n">
         <v>4000</v>
       </c>
-      <c r="G38" s="0" t="n">
+      <c r="H38" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H38" s="0" t="s">
+      <c r="I38" s="0" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O39" s="0" t="s">
+      <c r="P39" s="0" t="s">
         <v>317</v>
       </c>
     </row>
@@ -8768,16 +8984,16 @@
       <c r="A40" s="0" t="s">
         <v>318</v>
       </c>
-      <c r="F40" s="0" t="n">
+      <c r="G40" s="0" t="n">
         <v>10000</v>
       </c>
-      <c r="G40" s="0" t="n">
+      <c r="H40" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="H40" s="0" t="s">
+      <c r="I40" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="O40" s="13"/>
+      <c r="P40" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
@@ -8788,25 +9004,25 @@
       <c r="A43" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="F43" s="0" t="n">
+      <c r="G43" s="0" t="n">
         <v>5000</v>
       </c>
-      <c r="G43" s="0" t="n">
+      <c r="H43" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="H43" s="0" t="s">
+      <c r="I43" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="I43" s="0" t="n">
+      <c r="J43" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="J43" s="0" t="n">
+      <c r="K43" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="O43" s="0" t="s">
+      <c r="P43" s="0" t="s">
         <v>317</v>
       </c>
-      <c r="P43" s="0" t="s">
+      <c r="Q43" s="0" t="s">
         <v>321</v>
       </c>
     </row>
@@ -8814,16 +9030,16 @@
       <c r="A44" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="G44" s="0" t="n">
+      <c r="H44" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="H44" s="0" t="s">
+      <c r="I44" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="O44" s="0" t="s">
+      <c r="P44" s="0" t="s">
         <v>317</v>
       </c>
-      <c r="P44" s="0" t="s">
+      <c r="Q44" s="0" t="s">
         <v>322</v>
       </c>
     </row>
@@ -8831,13 +9047,13 @@
       <c r="A45" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="G45" s="0" t="n">
+      <c r="H45" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="H45" s="0" t="s">
+      <c r="I45" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="P45" s="0" t="s">
+      <c r="Q45" s="0" t="s">
         <v>323</v>
       </c>
     </row>
@@ -8845,13 +9061,13 @@
       <c r="A46" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="G46" s="0" t="s">
+      <c r="H46" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="H46" s="0" t="s">
+      <c r="I46" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="P46" s="0" t="s">
+      <c r="Q46" s="0" t="s">
         <v>326</v>
       </c>
     </row>
@@ -8859,19 +9075,19 @@
       <c r="A47" s="0" t="s">
         <v>327</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="D47" s="0" t="s">
         <v>328</v>
       </c>
-      <c r="G47" s="0" t="n">
+      <c r="H47" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="H47" s="0" t="s">
+      <c r="I47" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="O47" s="0" t="s">
+      <c r="P47" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="P47" s="0" t="s">
+      <c r="Q47" s="0" t="s">
         <v>329</v>
       </c>
     </row>
@@ -8879,10 +9095,10 @@
       <c r="A48" s="0" t="s">
         <v>330</v>
       </c>
-      <c r="H48" s="0" t="s">
+      <c r="I48" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="P48" s="0" t="s">
+      <c r="Q48" s="0" t="s">
         <v>331</v>
       </c>
     </row>
@@ -8895,13 +9111,13 @@
       <c r="A50" s="0" t="s">
         <v>333</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="D50" s="0" t="s">
         <v>334</v>
       </c>
-      <c r="H50" s="0" t="s">
+      <c r="I50" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="P50" s="0" t="s">
+      <c r="Q50" s="0" t="s">
         <v>335</v>
       </c>
     </row>
@@ -8909,13 +9125,13 @@
       <c r="A51" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="D51" s="0" t="s">
         <v>337</v>
       </c>
-      <c r="H51" s="0" t="s">
+      <c r="I51" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="P51" s="0" t="s">
+      <c r="Q51" s="0" t="s">
         <v>338</v>
       </c>
     </row>
@@ -8923,13 +9139,13 @@
       <c r="A52" s="0" t="s">
         <v>339</v>
       </c>
-      <c r="H52" s="0" t="s">
+      <c r="I52" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="I52" s="0" t="n">
+      <c r="J52" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="P52" s="0" t="s">
+      <c r="Q52" s="0" t="s">
         <v>340</v>
       </c>
     </row>
@@ -8937,13 +9153,13 @@
       <c r="A53" s="0" t="s">
         <v>341</v>
       </c>
-      <c r="H53" s="0" t="s">
+      <c r="I53" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="I53" s="0" t="n">
+      <c r="J53" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="P53" s="0" t="s">
+      <c r="Q53" s="0" t="s">
         <v>342</v>
       </c>
     </row>
@@ -8951,16 +9167,16 @@
       <c r="A54" s="0" t="s">
         <v>343</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="D54" s="0" t="s">
         <v>344</v>
       </c>
-      <c r="H54" s="0" t="s">
+      <c r="I54" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="O54" s="0" t="s">
+      <c r="P54" s="0" t="s">
         <v>317</v>
       </c>
-      <c r="P54" s="0" t="s">
+      <c r="Q54" s="0" t="s">
         <v>345</v>
       </c>
     </row>
@@ -8968,19 +9184,19 @@
       <c r="A56" s="0" t="s">
         <v>346</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="D56" s="0" t="s">
         <v>347</v>
       </c>
-      <c r="G56" s="0" t="s">
+      <c r="H56" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="H56" s="0" t="s">
+      <c r="I56" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="O56" s="0" t="s">
+      <c r="P56" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="P56" s="0" t="s">
+      <c r="Q56" s="0" t="s">
         <v>348</v>
       </c>
     </row>
@@ -8988,16 +9204,16 @@
       <c r="A57" s="0" t="s">
         <v>349</v>
       </c>
-      <c r="F57" s="0" t="n">
+      <c r="G57" s="0" t="n">
         <v>2945</v>
       </c>
-      <c r="H57" s="0" t="s">
+      <c r="I57" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="O57" s="0" t="s">
+      <c r="P57" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="P57" s="0" t="s">
+      <c r="Q57" s="0" t="s">
         <v>350</v>
       </c>
     </row>
@@ -9005,10 +9221,10 @@
       <c r="A58" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="H58" s="0" t="s">
+      <c r="I58" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="O58" s="0" t="s">
+      <c r="P58" s="0" t="s">
         <v>306</v>
       </c>
     </row>
@@ -9016,19 +9232,19 @@
       <c r="A60" s="0" t="s">
         <v>352</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="D60" s="0" t="s">
         <v>353</v>
       </c>
-      <c r="G60" s="0" t="s">
+      <c r="H60" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="H60" s="0" t="s">
+      <c r="I60" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="O60" s="0" t="s">
+      <c r="P60" s="0" t="s">
         <v>302</v>
       </c>
-      <c r="P60" s="0" t="s">
+      <c r="Q60" s="0" t="s">
         <v>354</v>
       </c>
     </row>
@@ -9036,16 +9252,16 @@
       <c r="A62" s="0" t="s">
         <v>355</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="D62" s="0" t="s">
         <v>356</v>
       </c>
-      <c r="G62" s="0" t="s">
+      <c r="H62" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="H62" s="0" t="s">
+      <c r="I62" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="P62" s="0" t="s">
+      <c r="Q62" s="0" t="s">
         <v>357</v>
       </c>
     </row>
@@ -9058,25 +9274,25 @@
       <c r="A65" s="0" t="s">
         <v>359</v>
       </c>
-      <c r="G65" s="0" t="n">
+      <c r="H65" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="H65" s="0" t="s">
+      <c r="I65" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="I65" s="0" t="n">
+      <c r="J65" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="J65" s="0" t="n">
+      <c r="K65" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="K65" s="0" t="n">
+      <c r="L65" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="O65" s="0" t="n">
+      <c r="P65" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="P65" s="0" t="s">
+      <c r="Q65" s="0" t="s">
         <v>360</v>
       </c>
     </row>
@@ -9084,13 +9300,13 @@
       <c r="A66" s="0" t="s">
         <v>361</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="D66" s="0" t="s">
         <v>362</v>
       </c>
-      <c r="O66" s="0" t="n">
+      <c r="P66" s="0" t="n">
         <v>0.005</v>
       </c>
-      <c r="P66" s="0" t="s">
+      <c r="Q66" s="0" t="s">
         <v>363</v>
       </c>
     </row>
@@ -9103,22 +9319,22 @@
       <c r="A69" s="0" t="s">
         <v>365</v>
       </c>
-      <c r="G69" s="0" t="n">
+      <c r="H69" s="0" t="n">
         <v>4</v>
-      </c>
-      <c r="I69" s="0" t="s">
-        <v>20</v>
       </c>
       <c r="J69" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="K69" s="0" t="n">
+      <c r="K69" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L69" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="O69" s="0" t="n">
+      <c r="P69" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="P69" s="0" t="s">
+      <c r="Q69" s="0" t="s">
         <v>366</v>
       </c>
     </row>
@@ -9126,13 +9342,13 @@
       <c r="A70" s="0" t="s">
         <v>367</v>
       </c>
-      <c r="G70" s="0" t="n">
+      <c r="H70" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K70" s="0" t="n">
+      <c r="L70" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="P70" s="0" t="s">
+      <c r="Q70" s="0" t="s">
         <v>368</v>
       </c>
     </row>
@@ -9140,13 +9356,13 @@
       <c r="A71" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="G71" s="0" t="n">
+      <c r="H71" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K71" s="0" t="n">
+      <c r="L71" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="P71" s="0" t="s">
+      <c r="Q71" s="0" t="s">
         <v>370</v>
       </c>
     </row>
@@ -9154,18 +9370,18 @@
       <c r="A72" s="0" t="s">
         <v>371</v>
       </c>
-      <c r="G72" s="0" t="s">
+      <c r="H72" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="K72" s="0" t="n">
+      <c r="L72" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="P72" s="0" t="s">
+      <c r="Q72" s="0" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K73" s="0" t="s">
+      <c r="L73" s="0" t="s">
         <v>373</v>
       </c>
     </row>
@@ -9173,13 +9389,13 @@
       <c r="A74" s="0" t="s">
         <v>374</v>
       </c>
-      <c r="C74" s="0" t="s">
+      <c r="D74" s="0" t="s">
         <v>375</v>
       </c>
-      <c r="K74" s="0" t="s">
+      <c r="L74" s="0" t="s">
         <v>376</v>
       </c>
-      <c r="P74" s="0" t="s">
+      <c r="Q74" s="0" t="s">
         <v>377</v>
       </c>
     </row>
@@ -9187,7 +9403,7 @@
       <c r="A75" s="0" t="s">
         <v>378</v>
       </c>
-      <c r="P75" s="0" t="s">
+      <c r="Q75" s="0" t="s">
         <v>379</v>
       </c>
     </row>
@@ -9200,16 +9416,16 @@
       <c r="A78" s="0" t="s">
         <v>381</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="C78" s="0" t="s">
         <v>382</v>
       </c>
-      <c r="F78" s="0" t="n">
+      <c r="G78" s="0" t="n">
         <v>50000</v>
       </c>
-      <c r="G78" s="0" t="s">
+      <c r="H78" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="K78" s="0" t="n">
+      <c r="L78" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9217,7 +9433,7 @@
       <c r="A79" s="0" t="s">
         <v>383</v>
       </c>
-      <c r="K79" s="0" t="n">
+      <c r="L79" s="0" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -9225,7 +9441,7 @@
       <c r="A80" s="0" t="s">
         <v>384</v>
       </c>
-      <c r="K80" s="0" t="n">
+      <c r="L80" s="0" t="n">
         <v>0.2</v>
       </c>
     </row>
@@ -9233,7 +9449,7 @@
       <c r="A81" s="0" t="s">
         <v>385</v>
       </c>
-      <c r="K81" s="0" t="n">
+      <c r="L81" s="0" t="n">
         <v>0.1</v>
       </c>
     </row>
@@ -9241,10 +9457,10 @@
       <c r="A82" s="0" t="s">
         <v>386</v>
       </c>
-      <c r="K82" s="0" t="n">
+      <c r="L82" s="0" t="n">
         <v>0.05</v>
       </c>
-      <c r="P82" s="0" t="s">
+      <c r="Q82" s="0" t="s">
         <v>387</v>
       </c>
     </row>
@@ -9252,10 +9468,10 @@
       <c r="A83" s="0" t="s">
         <v>388</v>
       </c>
-      <c r="C83" s="0" t="s">
+      <c r="D83" s="0" t="s">
         <v>389</v>
       </c>
-      <c r="F83" s="0" t="n">
+      <c r="G83" s="0" t="n">
         <v>10000</v>
       </c>
     </row>
@@ -9268,10 +9484,10 @@
       <c r="A86" s="0" t="s">
         <v>391</v>
       </c>
-      <c r="C86" s="0" t="s">
+      <c r="D86" s="0" t="s">
         <v>392</v>
       </c>
-      <c r="K86" s="0" t="n">
+      <c r="L86" s="0" t="n">
         <v>0.05</v>
       </c>
     </row>
@@ -9279,7 +9495,7 @@
       <c r="A87" s="0" t="s">
         <v>393</v>
       </c>
-      <c r="K87" s="0" t="n">
+      <c r="L87" s="0" t="n">
         <v>0.1</v>
       </c>
     </row>
@@ -9287,7 +9503,7 @@
       <c r="A88" s="0" t="s">
         <v>394</v>
       </c>
-      <c r="K88" s="0" t="n">
+      <c r="L88" s="0" t="n">
         <v>0.02</v>
       </c>
     </row>
@@ -9300,16 +9516,16 @@
       <c r="A91" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="B91" s="7" t="s">
+      <c r="C91" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="D91" s="7" t="s">
         <v>398</v>
       </c>
-      <c r="F91" s="7" t="n">
+      <c r="G91" s="7" t="n">
         <v>10000</v>
       </c>
-      <c r="G91" s="7" t="n">
+      <c r="H91" s="7" t="n">
         <v>4</v>
       </c>
     </row>
@@ -9317,19 +9533,21 @@
       <c r="A92" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="F92" s="7" t="n">
+      <c r="C92" s="0"/>
+      <c r="D92" s="0"/>
+      <c r="G92" s="7" t="n">
         <v>50000</v>
       </c>
-      <c r="G92" s="7" t="s">
+      <c r="H92" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="K92" s="7" t="n">
+      <c r="L92" s="7" t="n">
         <v>0.02</v>
       </c>
-      <c r="O92" s="7" t="n">
+      <c r="P92" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="P92" s="7" t="s">
+      <c r="Q92" s="7" t="s">
         <v>400</v>
       </c>
     </row>
@@ -9337,13 +9555,17 @@
       <c r="A93" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="K93" s="7" t="n">
+      <c r="C93" s="0"/>
+      <c r="D93" s="0"/>
+      <c r="G93" s="0"/>
+      <c r="H93" s="0"/>
+      <c r="L93" s="7" t="n">
         <v>0.05</v>
       </c>
-      <c r="O93" s="7" t="n">
+      <c r="P93" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="P93" s="7" t="s">
+      <c r="Q93" s="7" t="s">
         <v>402</v>
       </c>
     </row>
@@ -9351,13 +9573,17 @@
       <c r="A94" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="K94" s="7" t="n">
+      <c r="C94" s="0"/>
+      <c r="D94" s="0"/>
+      <c r="G94" s="0"/>
+      <c r="H94" s="0"/>
+      <c r="L94" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="O94" s="7" t="n">
+      <c r="P94" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="P94" s="7" t="s">
+      <c r="Q94" s="7" t="s">
         <v>404</v>
       </c>
     </row>
@@ -9365,316 +9591,411 @@
       <c r="A95" s="7" t="s">
         <v>405</v>
       </c>
-      <c r="C95" s="7" t="s">
+      <c r="C95" s="0"/>
+      <c r="D95" s="7" t="s">
         <v>406</v>
       </c>
-      <c r="K95" s="7" t="n">
+      <c r="G95" s="0"/>
+      <c r="H95" s="0"/>
+      <c r="L95" s="7" t="n">
         <v>0.02</v>
       </c>
-      <c r="O95" s="7" t="n">
+      <c r="P95" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="P95" s="7" t="s">
+      <c r="Q95" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="Q95" s="7" t="s">
+      <c r="R95" s="7" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="96" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="96" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0"/>
+      <c r="B96" s="0"/>
+      <c r="C96" s="0"/>
+      <c r="D96" s="0"/>
+      <c r="G96" s="0"/>
+      <c r="H96" s="0"/>
+      <c r="L96" s="0"/>
+      <c r="P96" s="0"/>
+      <c r="Q96" s="0"/>
+      <c r="R96" s="0"/>
+    </row>
     <row r="97" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="7" t="s">
         <v>409</v>
       </c>
-      <c r="B97" s="7" t="s">
+      <c r="B97" s="0"/>
+      <c r="C97" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="C97" s="7" t="s">
+      <c r="D97" s="7" t="s">
         <v>411</v>
       </c>
-      <c r="F97" s="7" t="n">
+      <c r="G97" s="7" t="n">
         <v>20000</v>
       </c>
-      <c r="K97" s="7" t="n">
+      <c r="H97" s="0"/>
+      <c r="L97" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="O97" s="7" t="n">
+      <c r="P97" s="7" t="n">
         <v>0.0005</v>
       </c>
+      <c r="Q97" s="0"/>
+      <c r="R97" s="0"/>
     </row>
     <row r="98" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="7" t="s">
         <v>412</v>
       </c>
-      <c r="C98" s="7" t="s">
+      <c r="B98" s="0"/>
+      <c r="C98" s="0"/>
+      <c r="D98" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="F98" s="7" t="n">
+      <c r="G98" s="7" t="n">
         <v>50000</v>
       </c>
-      <c r="K98" s="7" t="n">
+      <c r="H98" s="0"/>
+      <c r="L98" s="7" t="n">
         <v>0.05</v>
       </c>
-      <c r="O98" s="7" t="n">
+      <c r="P98" s="7" t="n">
         <v>0.0005</v>
       </c>
-    </row>
-    <row r="99" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="Q98" s="0"/>
+      <c r="R98" s="0"/>
+    </row>
+    <row r="99" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0"/>
+      <c r="B99" s="0"/>
+      <c r="C99" s="0"/>
+      <c r="D99" s="0"/>
+      <c r="G99" s="0"/>
+      <c r="H99" s="0"/>
+      <c r="L99" s="0"/>
+      <c r="P99" s="0"/>
+      <c r="Q99" s="0"/>
+      <c r="R99" s="0"/>
+    </row>
     <row r="100" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="C100" s="7" t="s">
+      <c r="B100" s="0"/>
+      <c r="C100" s="0"/>
+      <c r="D100" s="7" t="s">
         <v>415</v>
       </c>
-      <c r="F100" s="7" t="n">
+      <c r="G100" s="7" t="n">
         <v>50000</v>
       </c>
-      <c r="K100" s="7" t="n">
+      <c r="H100" s="0"/>
+      <c r="L100" s="7" t="n">
         <v>0.03</v>
       </c>
-      <c r="O100" s="7" t="n">
+      <c r="P100" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="P100" s="7" t="s">
+      <c r="Q100" s="7" t="s">
         <v>416</v>
       </c>
+      <c r="R100" s="0"/>
     </row>
     <row r="101" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="7" t="s">
         <v>417</v>
       </c>
-      <c r="F101" s="7" t="n">
+      <c r="B101" s="0"/>
+      <c r="C101" s="0"/>
+      <c r="D101" s="0"/>
+      <c r="G101" s="7" t="n">
         <v>50000</v>
       </c>
-      <c r="K101" s="7" t="n">
+      <c r="H101" s="0"/>
+      <c r="L101" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="O101" s="7" t="n">
+      <c r="P101" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="P101" s="7" t="s">
+      <c r="Q101" s="7" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="102" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="103" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R101" s="0"/>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E102" s="7"/>
+      <c r="F102" s="7"/>
+      <c r="I102" s="7"/>
+      <c r="J102" s="7"/>
+      <c r="K102" s="7"/>
+      <c r="M102" s="7"/>
+      <c r="N102" s="7"/>
+      <c r="O102" s="7"/>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="7" t="s">
         <v>419</v>
       </c>
-      <c r="K103" s="7" t="n">
+      <c r="E103" s="7"/>
+      <c r="F103" s="7"/>
+      <c r="I103" s="7"/>
+      <c r="J103" s="7"/>
+      <c r="K103" s="7"/>
+      <c r="L103" s="7" t="n">
         <v>0.02</v>
       </c>
-      <c r="O103" s="7" t="n">
+      <c r="M103" s="7"/>
+      <c r="N103" s="7"/>
+      <c r="O103" s="7"/>
+      <c r="P103" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="P103" s="7" t="s">
+      <c r="Q103" s="7" t="s">
         <v>420</v>
       </c>
-      <c r="Q103" s="7" t="s">
+      <c r="R103" s="7" t="s">
         <v>421</v>
       </c>
-      <c r="R103" s="7" t="s">
+      <c r="S103" s="7" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="104" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="7" t="s">
         <v>423</v>
       </c>
-      <c r="K104" s="7" t="n">
+      <c r="E104" s="7"/>
+      <c r="F104" s="7"/>
+      <c r="I104" s="7"/>
+      <c r="J104" s="7"/>
+      <c r="K104" s="7"/>
+      <c r="L104" s="7" t="n">
         <v>0.05</v>
       </c>
-      <c r="O104" s="7" t="n">
+      <c r="M104" s="7"/>
+      <c r="N104" s="7"/>
+      <c r="O104" s="7"/>
+      <c r="P104" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="P104" s="7" t="s">
+      <c r="Q104" s="7" t="s">
         <v>424</v>
       </c>
-      <c r="Q104" s="7" t="s">
+      <c r="R104" s="7" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="105" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="K105" s="7" t="n">
+      <c r="E105" s="7"/>
+      <c r="F105" s="7"/>
+      <c r="I105" s="7"/>
+      <c r="J105" s="7"/>
+      <c r="K105" s="7"/>
+      <c r="L105" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="O105" s="7" t="n">
+      <c r="M105" s="7"/>
+      <c r="N105" s="7"/>
+      <c r="O105" s="7"/>
+      <c r="P105" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="P105" s="7" t="s">
+      <c r="Q105" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="Q105" s="7" t="s">
+      <c r="R105" s="7" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="106" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="K106" s="7" t="n">
+      <c r="E106" s="7"/>
+      <c r="F106" s="7"/>
+      <c r="I106" s="7"/>
+      <c r="J106" s="7"/>
+      <c r="K106" s="7"/>
+      <c r="L106" s="7" t="n">
         <v>0.2</v>
       </c>
-      <c r="O106" s="7" t="n">
+      <c r="M106" s="7"/>
+      <c r="N106" s="7"/>
+      <c r="O106" s="7"/>
+      <c r="P106" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="P106" s="7" t="s">
+      <c r="Q106" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="Q106" s="7" t="s">
+      <c r="R106" s="7" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="107" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="108" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E107" s="7"/>
+      <c r="F107" s="7"/>
+      <c r="I107" s="7"/>
+      <c r="J107" s="7"/>
+      <c r="K107" s="7"/>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="7" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="109" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E108" s="7"/>
+      <c r="F108" s="7"/>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="7" t="s">
         <v>433</v>
       </c>
-      <c r="F109" s="7" t="n">
+      <c r="E109" s="7"/>
+      <c r="F109" s="7"/>
+      <c r="G109" s="7" t="n">
         <v>100000</v>
       </c>
-      <c r="G109" s="7" t="s">
+      <c r="H109" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="K109" s="7" t="n">
+      <c r="L109" s="7" t="n">
         <v>0.02</v>
       </c>
     </row>
-    <row r="110" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="111" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="112" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="7" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="113" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="G113" s="7" t="s">
+      <c r="H113" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="K113" s="7" t="n">
+      <c r="L113" s="7" t="n">
         <v>0.002</v>
       </c>
-      <c r="O113" s="7" t="n">
+      <c r="P113" s="7" t="n">
         <v>0.001</v>
       </c>
     </row>
-    <row r="114" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="7" t="s">
         <v>436</v>
       </c>
-      <c r="K114" s="7" t="n">
+      <c r="L114" s="7" t="n">
         <v>0.005</v>
       </c>
-      <c r="O114" s="7" t="n">
+      <c r="P114" s="7" t="n">
         <v>0.0005</v>
       </c>
     </row>
-    <row r="115" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="7" t="s">
         <v>437</v>
       </c>
-      <c r="K115" s="7" t="n">
+      <c r="L115" s="7" t="n">
         <v>0.001</v>
       </c>
-      <c r="O115" s="7" t="n">
+      <c r="P115" s="7" t="n">
         <v>0.001</v>
       </c>
     </row>
-    <row r="116" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="7" t="s">
         <v>438</v>
       </c>
-      <c r="K116" s="7" t="n">
+      <c r="L116" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="O116" s="7" t="n">
+      <c r="P116" s="7" t="n">
         <v>0.001</v>
       </c>
     </row>
-    <row r="117" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="K117" s="7" t="n">
+      <c r="L117" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="O117" s="7" t="n">
+      <c r="P117" s="7" t="n">
         <v>0.0005</v>
       </c>
     </row>
-    <row r="118" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="7" t="s">
         <v>440</v>
       </c>
-      <c r="K118" s="7" t="n">
+      <c r="L118" s="7" t="n">
         <v>0.0001</v>
       </c>
-      <c r="O118" s="7" t="n">
+      <c r="P118" s="7" t="n">
         <v>0.0005</v>
       </c>
     </row>
-    <row r="119" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="7" t="s">
         <v>441</v>
       </c>
-      <c r="K119" s="7" t="n">
+      <c r="L119" s="7" t="n">
         <v>0.0005</v>
       </c>
-      <c r="O119" s="7" t="n">
+      <c r="P119" s="7" t="n">
         <v>0.0001</v>
       </c>
     </row>
-    <row r="120" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="121" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="7" t="s">
         <v>442</v>
       </c>
-      <c r="C121" s="7" t="s">
+      <c r="B121" s="7"/>
+      <c r="D121" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="K121" s="7" t="n">
+      <c r="L121" s="7" t="n">
         <v>0.02</v>
       </c>
-      <c r="O121" s="7" t="n">
+      <c r="P121" s="7" t="n">
         <v>0.0005</v>
       </c>
     </row>
-    <row r="122" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="C122" s="7" t="s">
+      <c r="B122" s="7"/>
+      <c r="D122" s="7" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="123" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="7" t="s">
         <v>446</v>
       </c>
-      <c r="K123" s="7" t="n">
+      <c r="B123" s="7"/>
+      <c r="L123" s="7" t="n">
         <v>0.05</v>
       </c>
-      <c r="O123" s="7" t="n">
+      <c r="P123" s="7" t="n">
         <v>0.0005</v>
       </c>
     </row>
-    <row r="124" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="7" t="s">
         <v>447</v>
       </c>
-      <c r="C124" s="7" t="s">
+      <c r="B124" s="7"/>
+      <c r="D124" s="7" t="s">
         <v>448</v>
       </c>
     </row>
@@ -9687,22 +10008,22 @@
       <c r="A127" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="C127" s="0" t="s">
+      <c r="D127" s="0" t="s">
         <v>451</v>
       </c>
-      <c r="F127" s="0" t="n">
+      <c r="G127" s="0" t="n">
         <v>100000</v>
       </c>
-      <c r="G127" s="0" t="n">
+      <c r="H127" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="J127" s="0" t="n">
+      <c r="K127" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="K127" s="0" t="n">
+      <c r="L127" s="0" t="n">
         <v>0.02</v>
       </c>
-      <c r="O127" s="0" t="n">
+      <c r="P127" s="0" t="n">
         <v>0.0005</v>
       </c>
     </row>
@@ -9710,16 +10031,16 @@
       <c r="A128" s="0" t="s">
         <v>452</v>
       </c>
-      <c r="G128" s="0" t="n">
+      <c r="H128" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="J128" s="0" t="n">
+      <c r="K128" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="K128" s="0" t="n">
+      <c r="L128" s="0" t="n">
         <v>0.02</v>
       </c>
-      <c r="O128" s="0" t="n">
+      <c r="P128" s="0" t="n">
         <v>0.0005</v>
       </c>
     </row>
@@ -9727,16 +10048,16 @@
       <c r="A129" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="C129" s="0" t="s">
+      <c r="D129" s="0" t="s">
         <v>454</v>
       </c>
-      <c r="G129" s="0" t="n">
+      <c r="H129" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="J129" s="0" t="n">
+      <c r="K129" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="P129" s="0" t="s">
+      <c r="Q129" s="0" t="s">
         <v>455</v>
       </c>
     </row>
@@ -9744,7 +10065,7 @@
       <c r="A130" s="0" t="s">
         <v>456</v>
       </c>
-      <c r="J130" s="0" t="n">
+      <c r="K130" s="0" t="n">
         <v>0.02</v>
       </c>
     </row>
@@ -9752,22 +10073,22 @@
       <c r="A135" s="0" t="s">
         <v>457</v>
       </c>
-      <c r="E135" s="0" t="s">
+      <c r="F135" s="0" t="s">
         <v>458</v>
       </c>
-      <c r="F135" s="0" t="n">
+      <c r="G135" s="0" t="n">
         <v>10000</v>
       </c>
-      <c r="G135" s="0" t="s">
+      <c r="H135" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="K135" s="0" t="n">
+      <c r="L135" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="N135" s="0" t="n">
+      <c r="O135" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="O135" s="0" t="n">
+      <c r="P135" s="0" t="n">
         <v>0.01</v>
       </c>
     </row>
@@ -9775,7 +10096,7 @@
       <c r="A136" s="0" t="s">
         <v>459</v>
       </c>
-      <c r="K136" s="0" t="n">
+      <c r="L136" s="0" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9783,15 +10104,15 @@
       <c r="A137" s="0" t="s">
         <v>460</v>
       </c>
-      <c r="K137" s="0" t="n">
+      <c r="L137" s="0" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K141" s="0" t="n">
+      <c r="L141" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="O141" s="0" t="n">
+      <c r="P141" s="0" t="n">
         <v>0.01</v>
       </c>
     </row>
@@ -9799,16 +10120,16 @@
       <c r="A142" s="0" t="s">
         <v>461</v>
       </c>
-      <c r="C142" s="0" t="s">
+      <c r="D142" s="0" t="s">
         <v>462</v>
       </c>
-      <c r="G142" s="0" t="s">
+      <c r="H142" s="0" t="s">
         <v>325</v>
       </c>
-      <c r="K142" s="0" t="n">
+      <c r="L142" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O142" s="0" t="n">
+      <c r="P142" s="0" t="n">
         <v>0.01</v>
       </c>
     </row>
@@ -9816,13 +10137,13 @@
       <c r="A143" s="0" t="s">
         <v>463</v>
       </c>
-      <c r="E143" s="0" t="s">
+      <c r="F143" s="0" t="s">
         <v>464</v>
       </c>
-      <c r="F143" s="0" t="n">
+      <c r="G143" s="0" t="n">
         <v>100000</v>
       </c>
-      <c r="K143" s="0" t="n">
+      <c r="L143" s="0" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9830,10 +10151,10 @@
       <c r="A144" s="0" t="s">
         <v>465</v>
       </c>
-      <c r="K144" s="0" t="n">
+      <c r="L144" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="O144" s="0" t="n">
+      <c r="P144" s="0" t="n">
         <v>0.002</v>
       </c>
     </row>
@@ -9841,7 +10162,7 @@
       <c r="A145" s="0" t="s">
         <v>466</v>
       </c>
-      <c r="K145" s="0" t="n">
+      <c r="L145" s="0" t="n">
         <v>5</v>
       </c>
     </row>
@@ -9849,8 +10170,169 @@
       <c r="A146" s="0" t="s">
         <v>467</v>
       </c>
-      <c r="K146" s="0" t="n">
+      <c r="L146" s="0" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="D149" s="0" t="s">
+        <v>470</v>
+      </c>
+      <c r="H149" s="0" t="s">
+        <v>471</v>
+      </c>
+      <c r="P149" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="Q149" s="0" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="H150" s="0" t="s">
+        <v>474</v>
+      </c>
+      <c r="P150" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="Q150" s="0" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="H151" s="0" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="P154" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="Q154" s="0" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="R154" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>483</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="Q157" s="0" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1"/>
+    </row>
+    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="L162" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="P162" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>489</v>
+      </c>
+      <c r="L163" s="0" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>490</v>
+      </c>
+      <c r="L164" s="0" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>491</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="L166" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="P166" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="L167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P167" s="0" t="n">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="P168" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="R168" s="0" t="s">
+        <v>495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>